<commit_message>
more edits to xlsx, images + added new part to L2
</commit_message>
<xml_diff>
--- a/xlsx/L2-2.xlsx
+++ b/xlsx/L2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\QI-104\IHI-QI104\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBEA0B-F7C3-4243-9D9B-C6AFF06AC001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C347D1E7-AEAF-4B3E-8EDC-8F9C93272FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Week</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>median</t>
-  </si>
-  <si>
-    <t>baseline</t>
   </si>
 </sst>
 </file>
@@ -566,91 +563,91 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17.406714297322196</c:v>
+                  <c:v>17.225503982499525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,91 +789,91 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.2752744720077462</c:v>
+                  <c:v>3.0940641571850751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -897,7 +894,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>baseline</c:v>
+                  <c:v>median</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1018,91 +1015,91 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.153041308968742</c:v>
+                  <c:v>10.159784069842299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2125,13 +2122,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
+      <xdr:colOff>430694</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>434579</xdr:colOff>
+      <xdr:colOff>434578</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -2148,8 +2145,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11406187" y="2590800"/>
-          <a:ext cx="636986" cy="238125"/>
+          <a:off x="11529390" y="2590800"/>
+          <a:ext cx="616797" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2177,7 +2174,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="1"/>
-            <a:t>Baseline</a:t>
+            <a:t>Median</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -3444,7 +3441,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3477,16 +3474,16 @@
         <v>10.153041308968742</v>
       </c>
       <c r="C2" s="1">
-        <f>B2</f>
-        <v>10.153041308968742</v>
+        <f>MEDIAN(B2:B30)</f>
+        <v>10.159784069842299</v>
       </c>
       <c r="D2" s="1">
         <f>H$3+(H$2* 3 )</f>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E2" s="1">
         <f>H$3-(H$2* 3 )</f>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -3505,21 +3502,22 @@
       </c>
       <c r="C3" s="1">
         <f>C$2</f>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D53" si="0">H$3+(H$2* 3 )</f>
-        <v>17.406714297322196</v>
+        <f t="shared" ref="D3:D30" si="0">H$3+(H$2* 3 )</f>
+        <v>17.225503982499525</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E53" si="1">H$3-(H$2* 3 )</f>
-        <v>3.2752744720077462</v>
+        <f t="shared" ref="E3:E30" si="1">H$3-(H$2* 3 )</f>
+        <v>3.0940641571850751</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>10.34099438466497</v>
+      <c r="H3" s="1">
+        <f>MEDIAN(B2:B30)</f>
+        <v>10.159784069842299</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3531,15 +3529,15 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:C30" si="2">C$2</f>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3551,15 +3549,15 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3571,15 +3569,15 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3591,15 +3589,15 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3611,15 +3609,15 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3631,15 +3629,15 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3651,15 +3649,15 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3671,15 +3669,15 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3691,15 +3689,15 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3711,15 +3709,15 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3731,15 +3729,15 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3751,15 +3749,15 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3771,15 +3769,15 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3791,15 +3789,15 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,15 +3809,15 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3831,15 +3829,15 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3851,15 +3849,15 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3871,15 +3869,15 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3891,15 +3889,15 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,15 +3909,15 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3931,15 +3929,15 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3951,15 +3949,15 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,15 +3969,15 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3991,15 +3989,15 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4011,15 +4009,15 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4031,15 +4029,15 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4051,15 +4049,15 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="2"/>
-        <v>10.153041308968742</v>
+        <v>10.159784069842299</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>17.406714297322196</v>
+        <v>17.225503982499525</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="1"/>
-        <v>3.2752744720077462</v>
+        <v>3.0940641571850751</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added missing circle to chart L2-2
</commit_message>
<xml_diff>
--- a/xlsx/L2-2.xlsx
+++ b/xlsx/L2-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\QI-104\IHI-QI104\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79790DE8-3F84-40B5-9A3B-7338A8111E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA85410-821B-4CE2-80A9-B79EE3E8A1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3049,13 +3049,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>204389</xdr:colOff>
+      <xdr:colOff>213914</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>171757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>409088</xdr:colOff>
+      <xdr:colOff>396794</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>176007</xdr:rowOff>
     </xdr:to>
@@ -3072,8 +3072,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7012693" y="2648257"/>
-          <a:ext cx="204699" cy="194750"/>
+          <a:off x="6986189" y="2648257"/>
+          <a:ext cx="182880" cy="194750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3117,13 +3117,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>298811</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>175070</xdr:rowOff>
+      <xdr:rowOff>165545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>503510</xdr:colOff>
+      <xdr:colOff>481691</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>179320</xdr:rowOff>
+      <xdr:rowOff>169795</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3138,8 +3138,74 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8945854" y="2651570"/>
-          <a:ext cx="204699" cy="194750"/>
+          <a:off x="8899886" y="2642045"/>
+          <a:ext cx="182880" cy="194750"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>497593</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>70873</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Oval 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FCE76F-5E3B-4B46-8027-6CC50E1DCBB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6050668" y="2648257"/>
+          <a:ext cx="182880" cy="194750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3447,7 +3513,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>